<commit_message>
lisibility improvements based on the review
</commit_message>
<xml_diff>
--- a/SchemaDispositifAide.xlsx
+++ b/SchemaDispositifAide.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Porteur.s de l'aide*</t>
   </si>
   <si>
-    <t xml:space="preserve">SIREN du porteur</t>
+    <t xml:space="preserve">SIREN du.es porteur.s</t>
   </si>
   <si>
     <t xml:space="preserve">Bénéficiaire.s de l'aide*</t>
@@ -230,7 +230,7 @@
     <t xml:space="preserve">duree_aide</t>
   </si>
   <si>
-    <t xml:space="preserve">projet_reference</t>
+    <t xml:space="preserve">projets_reference</t>
   </si>
   <si>
     <t xml:space="preserve">exemple_projet</t>
@@ -374,7 +374,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
-Titre court, nom commercial du dispositif. Si pas de titre commercial clairement identifé, un titre générique du type \"Dispositif { opérateur principal }\" peut être utilisé
+Titre court, nom commercial du dispositif. Si pas de titre commercial clairement identifé, un titre générique du type `Dispositif { opérateur principal }` peut être utilisé
 </t>
     </r>
     <r>
@@ -404,8 +404,30 @@
 - distinguer les offres les unes des autres.
 Formulation :
 - 6 à 15 mots.
-- La promesse commence par un verbe à l'impératif\n- rédigée sous l'angle du bénéfice utilisateur, s'adressant à lui par le pluriel de politesse \"vous\" \"votre entreprise\" 
-- pas de point à la fin de la promesse (sauf point d'exclamation)
+- La promesse commence par un verbe à l'impératif
+- rédigée sous l'angle du bénéfice utilisateur, s'adressant à lui par le pluriel de politesse </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">`vous` `votre entreprise`
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- pas de point à la fin de la promesse (sauf point d'exclamation)
 Texte limité à 180 caractères
 </t>
     </r>
@@ -421,32 +443,12 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Description courte de l'objectif du dispositif. Qu'est-ce que l'entreprise gagne à bénéficier de cette aide  ? 
+    <t xml:space="preserve">Description courte de l'objectif du dispositif. Qu'est-ce que l'entreprise gagne à bénéficier de cette aide  ? 
 Formulation : 
 - 40 à 60 mots 
-- rédigés sous l'angle du bénéfice utilisateur, s'adressant à lui par le pluriel de politesse "vous"/"votre entreprise"
+- rédigés sous l'angle du bénéfice utilisateur, s'adressant à lui par le pluriel de politesse `vous` `votre entreprise`
 - La description courte est ponctuée par un point.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Ex : L’ADEME soutient financièrement les entreprises qui souhaitent questionner leur modèle économique pour identifier un nouveau modèle compatible avec une trajectoire bas carbone. Vous serez accompagné avec la méthode ACT Pas à Pas (Assessing Low Carbon Transition), une méthode structurante, progressive et sur le long terme qui aide les entreprises à réduire significativement leurs émissions de gaz à effet de serre.</t>
-    </r>
+Ex : L’ADEME soutient financièrement les entreprises qui souhaitent questionner leur modèle économique pour identifier un nouveau modèle compatible avec une trajectoire bas carbone. Vous serez accompagné avec la méthode ACT Pas à Pas (Assessing Low Carbon Transition), une méthode structurante, progressive et sur le long terme qui aide les entreprises à réduire significativement leurs émissions de gaz à effet de serre.</t>
   </si>
   <si>
     <r>
@@ -516,7 +518,7 @@
       </rPr>
       <t xml:space="preserve">Nom du.des porteur.s de l'aide. 
 S'il y a plusieurs porteurs, mettre un pipe ( | ) sans espace entre les différents porteurs.
- Le premier porteur est considérer le porteur/opérateur principal de l'aide
+ Le premier porteur est considéré comme le porteur/opérateur principal de l'aide
 </t>
     </r>
     <r>
@@ -1137,28 +1139,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Couverture géographique exclues du dispositif d'aide.
- Champs à écrire en utilisant le formalisme du Code Officiel Géographique du COG : https://www.insee.fr/fr/information/5230987. Séparer chaque code COG par des </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">pipes</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">. Cette propriété a précédence sur les \"eligibilite_geographique\" s'il y a recouvrement.
+ Champs à écrire en utilisant le formalisme du Code Officiel Géographique du COG : https://www.insee.fr/fr/information/5230987. Séparer chaque code COG par des pipes. Cette propriété a précédence sur les \"eligibilite_geographique\" s'il y a recouvrement.
 </t>
     </r>
     <r>
@@ -1215,6 +1196,7 @@
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">pipes</t>
     </r>
@@ -1673,6 +1655,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -1687,13 +1676,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -2211,8 +2193,8 @@
   </sheetPr>
   <dimension ref="A1:AV1010"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2261,7 +2243,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="37.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="19.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="19.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>